<commit_message>
fixed xlsx and fixed read file
</commit_message>
<xml_diff>
--- a/app/src/main/assets/dars_v2.xlsx
+++ b/app/src/main/assets/dars_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>Code</t>
   </si>
@@ -46,7 +46,40 @@
     <t>БОЙМАТОВ Д.</t>
   </si>
   <si>
-    <t>Душанбе</t>
+    <t>ФИЗИКА- МАТЕМАТИКА</t>
+  </si>
+  <si>
+    <t>Пониделник</t>
+  </si>
+  <si>
+    <t>Вторник</t>
+  </si>
+  <si>
+    <t>9:00-10:50</t>
+  </si>
+  <si>
+    <t>10:00-11:50</t>
+  </si>
+  <si>
+    <t>11:00-11:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТАРБИЯИ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ҶИСМОНӢ</t>
+  </si>
+  <si>
+    <t>8:00-11:50</t>
+  </si>
+  <si>
+    <t>9:00-11:50</t>
+  </si>
+  <si>
+    <t>Физика</t>
+  </si>
+  <si>
+    <t>ФИЗИКА- Информатика</t>
   </si>
 </sst>
 </file>
@@ -385,21 +418,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="6" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -436,12 +469,12 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -456,7 +489,127 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>201</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>